<commit_message>
full mgrid on M1
</commit_message>
<xml_diff>
--- a/12_40CoreBench.xlsx
+++ b/12_40CoreBench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="smithwa" sheetId="12" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="101">
   <si>
     <t>12 Core Potsdam Bench measurements</t>
   </si>
@@ -330,6 +330,9 @@
   <si>
     <t>Mem 1,6 %</t>
   </si>
+  <si>
+    <t>Mem 0.4%</t>
+  </si>
 </sst>
 </file>
 
@@ -1355,11 +1358,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199983488"/>
-        <c:axId val="199985024"/>
+        <c:axId val="197659264"/>
+        <c:axId val="197677440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199983488"/>
+        <c:axId val="197659264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199985024"/>
+        <c:crossAx val="197677440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1377,7 +1380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199985024"/>
+        <c:axId val="197677440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199983488"/>
+        <c:crossAx val="197659264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2544,11 +2547,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="201155712"/>
-        <c:axId val="201157248"/>
+        <c:axId val="196893696"/>
+        <c:axId val="196915968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="201155712"/>
+        <c:axId val="196893696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201157248"/>
+        <c:crossAx val="196915968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2566,7 +2569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201157248"/>
+        <c:axId val="196915968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2577,7 +2580,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201155712"/>
+        <c:crossAx val="196893696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3204,11 +3207,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200040832"/>
-        <c:axId val="200042368"/>
+        <c:axId val="198195840"/>
+        <c:axId val="198209920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200040832"/>
+        <c:axId val="198195840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3218,7 +3221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200042368"/>
+        <c:crossAx val="198209920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3226,7 +3229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200042368"/>
+        <c:axId val="198209920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3237,7 +3240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200040832"/>
+        <c:crossAx val="198195840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3873,11 +3876,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200082176"/>
-        <c:axId val="200083712"/>
+        <c:axId val="198237184"/>
+        <c:axId val="198247168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200082176"/>
+        <c:axId val="198237184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3886,7 +3889,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200083712"/>
+        <c:crossAx val="198247168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3894,7 +3897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200083712"/>
+        <c:axId val="198247168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3905,7 +3908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200082176"/>
+        <c:crossAx val="198237184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4421,11 +4424,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200148096"/>
-        <c:axId val="200149632"/>
+        <c:axId val="198290816"/>
+        <c:axId val="198292608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200148096"/>
+        <c:axId val="198290816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4434,7 +4437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200149632"/>
+        <c:crossAx val="198292608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4442,7 +4445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200149632"/>
+        <c:axId val="198292608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4453,7 +4456,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200148096"/>
+        <c:crossAx val="198290816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5195,11 +5198,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200201728"/>
-        <c:axId val="200203264"/>
+        <c:axId val="198383488"/>
+        <c:axId val="198385024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200201728"/>
+        <c:axId val="198383488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5208,7 +5211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200203264"/>
+        <c:crossAx val="198385024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5216,7 +5219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200203264"/>
+        <c:axId val="198385024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5227,7 +5230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200201728"/>
+        <c:crossAx val="198383488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5763,11 +5766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200620288"/>
-        <c:axId val="200622080"/>
+        <c:axId val="198423680"/>
+        <c:axId val="198425216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200620288"/>
+        <c:axId val="198423680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5776,7 +5779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200622080"/>
+        <c:crossAx val="198425216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5784,7 +5787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200622080"/>
+        <c:axId val="198425216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5795,7 +5798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200620288"/>
+        <c:crossAx val="198423680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6094,11 +6097,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200668288"/>
-        <c:axId val="200669824"/>
+        <c:axId val="198516096"/>
+        <c:axId val="198546560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200668288"/>
+        <c:axId val="198516096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6107,7 +6110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200669824"/>
+        <c:crossAx val="198546560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6115,7 +6118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200669824"/>
+        <c:axId val="198546560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6126,7 +6129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200668288"/>
+        <c:crossAx val="198516096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6438,11 +6441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200825856"/>
-        <c:axId val="200831744"/>
+        <c:axId val="198571520"/>
+        <c:axId val="198573056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200825856"/>
+        <c:axId val="198571520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6451,7 +6454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200831744"/>
+        <c:crossAx val="198573056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6459,7 +6462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200831744"/>
+        <c:axId val="198573056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6470,7 +6473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200825856"/>
+        <c:crossAx val="198571520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7166,11 +7169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200891392"/>
-        <c:axId val="200930048"/>
+        <c:axId val="196720128"/>
+        <c:axId val="196721664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200891392"/>
+        <c:axId val="196720128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7179,7 +7182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200930048"/>
+        <c:crossAx val="196721664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7187,7 +7190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200930048"/>
+        <c:axId val="196721664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7198,7 +7201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200891392"/>
+        <c:crossAx val="196720128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7820,8 +7823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10713,8 +10716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11362,6 +11365,16 @@
       <c r="F36">
         <v>30</v>
       </c>
+      <c r="G36">
+        <v>3559</v>
+      </c>
+      <c r="H36">
+        <v>1.33</v>
+      </c>
+      <c r="I36">
+        <f>AVERAGE(G7/G36)</f>
+        <v>19.913177858949144</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37">
@@ -11762,8 +11775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11900,6 +11913,16 @@
       <c r="A11">
         <v>5</v>
       </c>
+      <c r="B11">
+        <v>10934</v>
+      </c>
+      <c r="C11">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="D11">
+        <f>AVERAGE(B7/B11)</f>
+        <v>3.802999817084324</v>
+      </c>
       <c r="F11">
         <v>5</v>
       </c>
@@ -11908,6 +11931,16 @@
       <c r="A12">
         <v>6</v>
       </c>
+      <c r="B12">
+        <v>9078</v>
+      </c>
+      <c r="C12">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(B7/B12)</f>
+        <v>4.5805243445692883</v>
+      </c>
       <c r="F12">
         <v>6</v>
       </c>
@@ -11916,6 +11949,16 @@
       <c r="A13">
         <v>7</v>
       </c>
+      <c r="B13">
+        <v>7502</v>
+      </c>
+      <c r="C13">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(B7/B13)</f>
+        <v>5.5427885897094109</v>
+      </c>
       <c r="F13">
         <v>7</v>
       </c>
@@ -11924,6 +11967,16 @@
       <c r="A14">
         <v>8</v>
       </c>
+      <c r="B14">
+        <v>7111</v>
+      </c>
+      <c r="C14">
+        <v>0.622</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(B7/B14)</f>
+        <v>5.8475601181268457</v>
+      </c>
       <c r="F14">
         <v>8</v>
       </c>
@@ -11932,6 +11985,16 @@
       <c r="A15">
         <v>9</v>
       </c>
+      <c r="B15">
+        <v>6256</v>
+      </c>
+      <c r="C15">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(B7/B15)</f>
+        <v>6.6467391304347823</v>
+      </c>
       <c r="F15">
         <v>9</v>
       </c>
@@ -11940,6 +12003,16 @@
       <c r="A16">
         <v>10</v>
       </c>
+      <c r="B16">
+        <v>6136</v>
+      </c>
+      <c r="C16">
+        <v>0.72</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(B7/B16)</f>
+        <v>6.7767275097783575</v>
+      </c>
       <c r="F16">
         <v>10</v>
       </c>
@@ -11958,6 +12031,16 @@
       <c r="A17">
         <v>11</v>
       </c>
+      <c r="B17">
+        <v>5892</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE(B7/B17)</f>
+        <v>7.0573659198913781</v>
+      </c>
       <c r="F17">
         <v>11</v>
       </c>
@@ -12312,6 +12395,16 @@
       </c>
       <c r="F36">
         <v>30</v>
+      </c>
+      <c r="G36">
+        <v>4992</v>
+      </c>
+      <c r="H36">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="I36">
+        <f>AVERAGE(G7/G36)</f>
+        <v>14.212940705128204</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -12713,8 +12806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView topLeftCell="C66" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13257,6 +13350,16 @@
     <row r="66" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F66">
         <v>60</v>
+      </c>
+      <c r="G66">
+        <v>7802</v>
+      </c>
+      <c r="H66">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="I66">
+        <f>AVERAGE(G7/G66)</f>
+        <v>5.2136631632914634</v>
       </c>
     </row>
     <row r="67" spans="6:9" x14ac:dyDescent="0.25">
@@ -15464,8 +15567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="BF14" sqref="BF14"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17086,7 +17189,7 @@
         <v>4.7692207792207792</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I32" si="5">(B25/12)</f>
+        <f t="shared" ref="I25:I33" si="5">(B25/12)</f>
         <v>0.88014092608570615</v>
       </c>
       <c r="J25">
@@ -17524,6 +17627,9 @@
       <c r="A33" t="s">
         <v>79</v>
       </c>
+      <c r="B33">
+        <v>7.0573659198913781</v>
+      </c>
       <c r="C33">
         <v>7.1226447413497773</v>
       </c>
@@ -17538,6 +17644,10 @@
       </c>
       <c r="H33">
         <v>8.7028045207199671</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>0.5881138266576148</v>
       </c>
       <c r="J33">
         <f t="shared" si="6"/>
@@ -17756,8 +17866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J103"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18967,17 +19077,16 @@
         <v>42</v>
       </c>
       <c r="B48">
-        <v>562</v>
+        <f>AVERAGE(562,591)</f>
+        <v>576.5</v>
       </c>
       <c r="C48">
-        <v>7.6</v>
+        <f>AVERAGE(7.62,7.6)</f>
+        <v>7.6099999999999994</v>
       </c>
       <c r="D48">
         <f>AVERAGE(B7/B48)</f>
-        <v>11.421708185053381</v>
-      </c>
-      <c r="E48">
-        <v>591</v>
+        <v>11.134431916738942</v>
       </c>
       <c r="F48">
         <v>42</v>
@@ -19830,8 +19939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20959,15 +21068,45 @@
       <c r="F52">
         <v>46</v>
       </c>
+      <c r="G52">
+        <v>1185</v>
+      </c>
+      <c r="H52">
+        <v>4.43</v>
+      </c>
+      <c r="I52">
+        <f>AVERAGE(G7/G52)</f>
+        <v>32.633755274261603</v>
+      </c>
     </row>
     <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>47</v>
       </c>
+      <c r="G53">
+        <v>1165</v>
+      </c>
+      <c r="H53">
+        <v>4.5</v>
+      </c>
+      <c r="I53">
+        <f>AVERAGE(G7/G53)</f>
+        <v>33.193991416309011</v>
+      </c>
     </row>
     <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>48</v>
+      </c>
+      <c r="G54">
+        <v>1180</v>
+      </c>
+      <c r="H54">
+        <v>4.45</v>
+      </c>
+      <c r="I54">
+        <f>AVERAGE(G7/G54)</f>
+        <v>32.772033898305082</v>
       </c>
     </row>
     <row r="55" spans="6:9" x14ac:dyDescent="0.25">
@@ -21269,7 +21408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -24609,8 +24748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24633,6 +24772,9 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -24867,6 +25009,16 @@
       <c r="F16">
         <v>10</v>
       </c>
+      <c r="G16">
+        <v>3581</v>
+      </c>
+      <c r="H16">
+        <v>1.96</v>
+      </c>
+      <c r="I16">
+        <f>AVERAGE(G7/G16)</f>
+        <v>9.6043004747277294</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -25057,6 +25209,16 @@
       <c r="F26">
         <v>20</v>
       </c>
+      <c r="G26">
+        <v>1839</v>
+      </c>
+      <c r="H26">
+        <v>3.82</v>
+      </c>
+      <c r="I26">
+        <f>AVERAGE(G7/G26)</f>
+        <v>18.702011963023381</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -25247,6 +25409,16 @@
       <c r="F36">
         <v>30</v>
       </c>
+      <c r="G36">
+        <v>1330</v>
+      </c>
+      <c r="H36">
+        <v>5.29</v>
+      </c>
+      <c r="I36">
+        <f>AVERAGE(G7/G36)</f>
+        <v>25.859398496240601</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37">
@@ -25447,6 +25619,16 @@
       <c r="F66">
         <v>60</v>
       </c>
+      <c r="G66">
+        <v>959</v>
+      </c>
+      <c r="H66">
+        <v>7.33</v>
+      </c>
+      <c r="I66">
+        <f>AVERAGE(G7/G66)</f>
+        <v>35.863399374348276</v>
+      </c>
     </row>
     <row r="67" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F67">
@@ -25508,14 +25690,16 @@
         <v>70</v>
       </c>
       <c r="G76">
-        <v>909</v>
+        <f>AVERAGE(909,916)</f>
+        <v>912.5</v>
       </c>
       <c r="H76">
-        <v>7.73</v>
+        <f>AVERAGE(7.73,7.68)</f>
+        <v>7.7050000000000001</v>
       </c>
       <c r="I76">
         <f>AVERAGE(G7/G76)</f>
-        <v>37.836083608360838</v>
+        <v>37.690958904109586</v>
       </c>
     </row>
     <row r="77" spans="6:9" x14ac:dyDescent="0.25">
@@ -25667,8 +25851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26418,82 +26602,92 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F50">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F51">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F52">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>8070</v>
+      </c>
+      <c r="H56">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="I56">
+        <f>AVERAGE(G7/G56)</f>
+        <v>13.165923172242875</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F60">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F61">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F62">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F63">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F64">
         <v>58</v>
       </c>
@@ -26727,8 +26921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27363,6 +27557,16 @@
       <c r="F36">
         <v>30</v>
       </c>
+      <c r="G36">
+        <v>3311</v>
+      </c>
+      <c r="H36">
+        <v>1.37</v>
+      </c>
+      <c r="I36">
+        <f>AVERAGE(G7/G36)</f>
+        <v>7.940199335548173</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37">
@@ -27602,6 +27806,16 @@
     <row r="76" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F76">
         <v>70</v>
+      </c>
+      <c r="G76">
+        <v>2329</v>
+      </c>
+      <c r="H76">
+        <v>1.95</v>
+      </c>
+      <c r="I76">
+        <f>AVERAGE(G7/G76)</f>
+        <v>11.288106483469301</v>
       </c>
     </row>
     <row r="77" spans="6:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added MD plus presentation
</commit_message>
<xml_diff>
--- a/12_40CoreBench.xlsx
+++ b/12_40CoreBench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="smithwa" sheetId="12" r:id="rId1"/>
@@ -1373,11 +1373,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141503104"/>
-        <c:axId val="141521280"/>
+        <c:axId val="191659392"/>
+        <c:axId val="191669376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141503104"/>
+        <c:axId val="191659392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141521280"/>
+        <c:crossAx val="191669376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +1395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141521280"/>
+        <c:axId val="191669376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141503104"/>
+        <c:crossAx val="191659392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2571,11 +2571,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140803072"/>
-        <c:axId val="140825344"/>
+        <c:axId val="192020480"/>
+        <c:axId val="192022016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140803072"/>
+        <c:axId val="192020480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2585,7 +2585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140825344"/>
+        <c:crossAx val="192022016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2593,7 +2593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140825344"/>
+        <c:axId val="192022016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2604,14 +2604,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140803072"/>
+        <c:crossAx val="192020480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3232,11 +3231,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142031488"/>
-        <c:axId val="142049664"/>
+        <c:axId val="192253312"/>
+        <c:axId val="192263296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142031488"/>
+        <c:axId val="192253312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3246,7 +3245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142049664"/>
+        <c:crossAx val="192263296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3254,7 +3253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142049664"/>
+        <c:axId val="192263296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,14 +3264,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142031488"/>
+        <c:crossAx val="192253312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3902,11 +3900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142068736"/>
-        <c:axId val="142082816"/>
+        <c:axId val="192180224"/>
+        <c:axId val="192181760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142068736"/>
+        <c:axId val="192180224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3915,7 +3913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142082816"/>
+        <c:crossAx val="192181760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3923,7 +3921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142082816"/>
+        <c:axId val="192181760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3934,14 +3932,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142068736"/>
+        <c:crossAx val="192180224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4451,11 +4448,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142130560"/>
-        <c:axId val="142132352"/>
+        <c:axId val="192283008"/>
+        <c:axId val="192284544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142130560"/>
+        <c:axId val="192283008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4464,7 +4461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142132352"/>
+        <c:crossAx val="192284544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4472,7 +4469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142132352"/>
+        <c:axId val="192284544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4483,14 +4480,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142130560"/>
+        <c:crossAx val="192283008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5229,11 +5225,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141766656"/>
-        <c:axId val="141768192"/>
+        <c:axId val="192313600"/>
+        <c:axId val="192315392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141766656"/>
+        <c:axId val="192313600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5242,7 +5238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141768192"/>
+        <c:crossAx val="192315392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5250,7 +5246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141768192"/>
+        <c:axId val="192315392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5261,7 +5257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141766656"/>
+        <c:crossAx val="192313600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5797,11 +5793,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141804672"/>
-        <c:axId val="141806208"/>
+        <c:axId val="192343040"/>
+        <c:axId val="191963904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141804672"/>
+        <c:axId val="192343040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5810,7 +5806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141806208"/>
+        <c:crossAx val="191963904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5818,7 +5814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141806208"/>
+        <c:axId val="191963904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5829,7 +5825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141804672"/>
+        <c:crossAx val="192343040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6131,11 +6127,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141835648"/>
-        <c:axId val="141857920"/>
+        <c:axId val="192018304"/>
+        <c:axId val="192019840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141835648"/>
+        <c:axId val="192018304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6144,7 +6140,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141857920"/>
+        <c:crossAx val="192019840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6152,7 +6148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141857920"/>
+        <c:axId val="192019840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,14 +6159,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141835648"/>
+        <c:crossAx val="192018304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6482,11 +6477,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141878784"/>
-        <c:axId val="141880320"/>
+        <c:axId val="190480384"/>
+        <c:axId val="190481920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141878784"/>
+        <c:axId val="190480384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6495,7 +6490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141880320"/>
+        <c:crossAx val="190481920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6503,7 +6498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141880320"/>
+        <c:axId val="190481920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6514,14 +6509,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141878784"/>
+        <c:crossAx val="190480384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7223,11 +7217,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140621312"/>
-        <c:axId val="140622848"/>
+        <c:axId val="190351616"/>
+        <c:axId val="190369792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140621312"/>
+        <c:axId val="190351616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7236,7 +7230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140622848"/>
+        <c:crossAx val="190369792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7244,7 +7238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140622848"/>
+        <c:axId val="190369792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7255,14 +7249,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140621312"/>
+        <c:crossAx val="190351616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11830,7 +11823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12:D17"/>
     </sheetView>
   </sheetViews>
@@ -12861,8 +12854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13304,6 +13297,16 @@
       <c r="A26">
         <v>20</v>
       </c>
+      <c r="B26">
+        <v>9157</v>
+      </c>
+      <c r="C26">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(B7/B26)</f>
+        <v>3.2899421207819155</v>
+      </c>
       <c r="F26">
         <v>20</v>
       </c>
@@ -13321,6 +13324,16 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
+      </c>
+      <c r="B27">
+        <v>8898</v>
+      </c>
+      <c r="C27">
+        <v>0.52</v>
+      </c>
+      <c r="D27">
+        <f>AVERAGE(B7/B27)</f>
+        <v>3.3857046527309507</v>
       </c>
       <c r="F27">
         <v>21</v>
@@ -18105,27 +18118,27 @@
         <v>7.4451009354997542</v>
       </c>
       <c r="I34">
-        <f>(B34/12)</f>
+        <f t="shared" ref="I34:J36" si="13">(B34/12)</f>
         <v>0.68051305130513062</v>
       </c>
       <c r="J34">
-        <f>(C34/12)</f>
+        <f t="shared" si="13"/>
         <v>0.67904616490030534</v>
       </c>
       <c r="L34">
-        <f t="shared" ref="L34:O35" si="13">(E34/12)</f>
+        <f t="shared" ref="L34:O35" si="14">(E34/12)</f>
         <v>0.74253584757415048</v>
       </c>
       <c r="M34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.76214717741935489</v>
       </c>
       <c r="N34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.78039843104872009</v>
       </c>
       <c r="O34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.62042507795831281</v>
       </c>
       <c r="P34" t="s">
@@ -18164,27 +18177,27 @@
         <v>8.7185861332297527</v>
       </c>
       <c r="I35">
-        <f>(B35/12)</f>
+        <f t="shared" si="13"/>
         <v>0.50181086519114693</v>
       </c>
       <c r="J35">
-        <f>(C35/12)</f>
+        <f t="shared" si="13"/>
         <v>0.55885867941440093</v>
       </c>
       <c r="L35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.71393129770992358</v>
       </c>
       <c r="M35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.72881355932203384</v>
       </c>
       <c r="N35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.7295241809672387</v>
       </c>
       <c r="O35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.72654884443581269</v>
       </c>
       <c r="P35" t="s">
@@ -18223,27 +18236,27 @@
         <v>4.132510288065844</v>
       </c>
       <c r="I36">
-        <f>(B36/12)</f>
+        <f t="shared" si="13"/>
         <v>0.1893288084464555</v>
       </c>
       <c r="J36">
-        <f>(C36/12)</f>
+        <f t="shared" si="13"/>
         <v>0.20308202556220678</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36" si="14">(E36/12)</f>
+        <f t="shared" ref="L36" si="15">(E36/12)</f>
         <v>0.2994036970781157</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36" si="15">(F36/12)</f>
+        <f t="shared" ref="M36" si="16">(F36/12)</f>
         <v>0.30913680581209207</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36" si="16">(G36/12)</f>
+        <f t="shared" ref="N36" si="17">(G36/12)</f>
         <v>0.31790553374699254</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36" si="17">(H36/12)</f>
+        <f t="shared" ref="O36" si="18">(H36/12)</f>
         <v>0.34437585733882031</v>
       </c>
       <c r="P36" t="s">

</xml_diff>